<commit_message>
testing if this works
</commit_message>
<xml_diff>
--- a/Ideas.xlsx
+++ b/Ideas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexb\Song-Writing-Helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Song-Writing-Helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED26963-2921-4835-96F4-1A07A8896C2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3D7E8D-9EF7-4CA3-A47A-23362301E51E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{A3A27B2A-FD11-473B-8EDA-782773C5BF39}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A3A27B2A-FD11-473B-8EDA-782773C5BF39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Idea</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Not Implimented</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="8">
     <dxf>
       <font>
         <b/>
@@ -142,6 +145,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7093D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFB1F38D"/>
         </patternFill>
       </fill>
@@ -185,66 +202,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFE78181"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7093D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF395A5"/>
         </patternFill>
       </fill>
       <border>
@@ -629,20 +586,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332CA337-36A7-438D-8BF7-57DDBC354AA6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.15625" customWidth="1"/>
-    <col min="2" max="2" width="47.734375" customWidth="1"/>
-    <col min="3" max="3" width="22.26171875" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="47.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -653,7 +610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="33.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="33.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -664,35 +621,40 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Not Implimented">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Not Implimented">
       <formula>NOT(ISERROR(SEARCH("Not Implimented",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Under Development">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Under Development">
       <formula>NOT(ISERROR(SEARCH("Under Development",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Under Development">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Under Development">
       <formula>NOT(ISERROR(SEARCH("Under Development",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Fixing Bugs">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fixing Bugs">
       <formula>NOT(ISERROR(SEARCH("Fixing Bugs",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>